<commit_message>
Change the fluctuation of faith bonuses from daily to weekly.
</commit_message>
<xml_diff>
--- a/DanalinOfWater/LangMod/EN/custom_sources.xlsx
+++ b/DanalinOfWater/LangMod/EN/custom_sources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Thing" sheetId="1" state="visible" r:id="rId3"/>
@@ -598,7 +598,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">ボーナスが毎日変わる</t>
+      <t xml:space="preserve">ボーナスが毎週変わる</t>
     </r>
     <r>
       <rPr>
@@ -628,7 +628,7 @@
         <family val="1"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">Bonus changes daily,Bonus increases as the </t>
+      <t xml:space="preserve">Bonus changes weekly,Bonus increases as the </t>
     </r>
     <r>
       <rPr>
@@ -2269,12 +2269,12 @@
   </sheetPr>
   <dimension ref="A1:BO908"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="topRight" activeCell="AV1" activeCellId="0" sqref="AV1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="AV4" activeCellId="0" sqref="AV4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -48134,7 +48134,7 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>

</xml_diff>

<commit_message>
Strengthen the performance of Danalin's Pets and Artifacts.
</commit_message>
<xml_diff>
--- a/DanalinOfWater/LangMod/EN/custom_sources.xlsx
+++ b/DanalinOfWater/LangMod/EN/custom_sources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Thing" sheetId="1" state="visible" r:id="rId3"/>
@@ -367,7 +367,7 @@
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">breathing/10,CHA/20,swimming/13,music/20,sculpture/15,jewelry/15,weaving/15,handicraft/12,fishing/6,carpentry/6,blacksmith/6,alchemy/6</t>
+    <t xml:space="preserve">breathing/10,CHA/20,swimming/13,music/30,sculpture/25,jewelry/25,weaving/25,handicraft/20,fishing/15,carpentry/15,blacksmith/15,alchemy/15</t>
   </si>
   <si>
     <t xml:space="preserve">0,0</t>
@@ -1036,7 +1036,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">breathing,seeInvisible,swimming/8</t>
+      <t xml:space="preserve">breathing,seeInvisible,swimming/12</t>
     </r>
   </si>
   <si>
@@ -1693,7 +1693,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2269,12 +2269,12 @@
   </sheetPr>
   <dimension ref="A1:BO908"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AV1" activeCellId="0" sqref="AV1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AV4" activeCellId="0" sqref="AV4"/>
+      <selection pane="bottomRight" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -48407,12 +48407,12 @@
   </sheetPr>
   <dimension ref="A1:XFD4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Grant the drown the undead tag.
</commit_message>
<xml_diff>
--- a/DanalinOfWater/LangMod/EN/custom_sources.xlsx
+++ b/DanalinOfWater/LangMod/EN/custom_sources.xlsx
@@ -994,7 +994,7 @@
     <t xml:space="preserve">Neutral</t>
   </si>
   <si>
-    <t xml:space="preserve">noPortrait</t>
+    <t xml:space="preserve">noPortrait,undead</t>
   </si>
   <si>
     <t xml:space="preserve">servant</t>
@@ -48408,11 +48408,11 @@
   <dimension ref="A1:XFD4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="U5" activeCellId="0" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>